<commit_message>
Reestructuració de la interficie i noves imatges
</commit_message>
<xml_diff>
--- a/GUI/Hores agost setembre.xlsx
+++ b/GUI/Hores agost setembre.xlsx
@@ -44,10 +44,10 @@
     <t>5h</t>
   </si>
   <si>
-    <t>3h centre 6 h casa</t>
-  </si>
-  <si>
     <t>Treball a casa de nit</t>
+  </si>
+  <si>
+    <t>3h centre 4h casa</t>
   </si>
 </sst>
 </file>
@@ -470,10 +470,10 @@
         <v>42619</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reestructats els fitxers i noves funcions
Noves funcions implementades. Per exemple, funcio per poder escriure un
log de totes les accions que es van fent.
</commit_message>
<xml_diff>
--- a/GUI/Hores agost setembre.xlsx
+++ b/GUI/Hores agost setembre.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>3h</t>
   </si>
@@ -44,10 +44,16 @@
     <t>5h</t>
   </si>
   <si>
-    <t>Treball a casa de nit</t>
-  </si>
-  <si>
-    <t>3h centre 4h casa</t>
+    <t>4h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5h </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3h </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -385,7 +391,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,152 +476,138 @@
         <v>42619</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42620</v>
       </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42621</v>
       </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42622</v>
       </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>42623</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42624</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42625</v>
       </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42626</v>
       </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42627</v>
       </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42628</v>
       </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>42629</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>42630</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>42631</v>
-      </c>
+      <c r="A21" s="4"/>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>42632</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>42633</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>42634</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>42635</v>
-      </c>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>42636</v>
-      </c>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>42637</v>
-      </c>
+      <c r="A27" s="4"/>
       <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>42638</v>
-      </c>
+      <c r="A28" s="4"/>
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>42639</v>
-      </c>
+      <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>42640</v>
-      </c>
+      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>42641</v>
-      </c>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>42642</v>
-      </c>
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>42643</v>
-      </c>
+      <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>42644</v>
-      </c>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>42645</v>
-      </c>
+      <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>42646</v>
-      </c>
+      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>